<commit_message>
Korean Air base; site unreliable
</commit_message>
<xml_diff>
--- a/CarrierPrefixes.xlsx
+++ b/CarrierPrefixes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
   <si>
     <t>Carrier</t>
   </si>
@@ -129,6 +129,12 @@
   </si>
   <si>
     <t>074</t>
+  </si>
+  <si>
+    <t>KoreanAir</t>
+  </si>
+  <si>
+    <t>180</t>
   </si>
 </sst>
 </file>
@@ -447,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B13" sqref="B13:B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,58 +567,69 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>27</v>
+        <v>36</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" s="1">
-        <v>157</v>
+        <v>11</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" t="s">
-        <v>28</v>
+        <v>23</v>
+      </c>
+      <c r="B16" s="1">
+        <v>157</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="C17" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>28</v>
       </c>
     </row>
@@ -623,7 +640,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B19:B20 B4 B5:B7 B9:B10 B11 B12:B18" numberStoredAsText="1"/>
+    <ignoredError sqref="B20 B4 B5:B7 B9:B10 B11 B12 B13:B19" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added urls to carrier list
</commit_message>
<xml_diff>
--- a/CarrierPrefixes.xlsx
+++ b/CarrierPrefixes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="61">
   <si>
     <t>Carrier</t>
   </si>
@@ -135,16 +135,96 @@
   </si>
   <si>
     <t>180</t>
+  </si>
+  <si>
+    <t>United</t>
+  </si>
+  <si>
+    <t>016</t>
+  </si>
+  <si>
+    <t>about 11% can't do/cant find</t>
+  </si>
+  <si>
+    <t>about 52% done/in progress/blocked</t>
+  </si>
+  <si>
+    <t>about 37% not looked at</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>https://www.airbridgecargo.com/en/tracking/</t>
+  </si>
+  <si>
+    <t>https://www.afklcargo.com/WW/en/local/app/index.jsp#/tntsinglesearch</t>
+  </si>
+  <si>
+    <t>https://www.airtahitinui.com/us-en/online-cargo-tracking</t>
+  </si>
+  <si>
+    <t>http://www.cathaypacificcargo.com/ManageYourShipment/TrackYourShipment/tabid/108/SingleAWBNo/160-05480334-/language/en-US/Default.aspx</t>
+  </si>
+  <si>
+    <t>https://cargo.china-airlines.com/CCNetv2/content/manage/ShipmentTracking.aspx?</t>
+  </si>
+  <si>
+    <t>https://aviationcargo.dhl.com/aviationcargo/track/</t>
+  </si>
+  <si>
+    <t>https://skychain.emirates.com/skychain/app?service=page/nwp:Trackshipmt&amp;amp;initial=y</t>
+  </si>
+  <si>
+    <t>http://www.brcargo.com/ec_web/Default.aspx?Parm2=191&amp;amp;Parm3=undefined</t>
+  </si>
+  <si>
+    <t>http://www.jal.co.jp/en/jalcargo/inter/awb/</t>
+  </si>
+  <si>
+    <t>https://lufthansa-cargo.com/eservices/etracking</t>
+  </si>
+  <si>
+    <t>https://cargo.koreanair.com/en/tracking?</t>
+  </si>
+  <si>
+    <t>http://www.maskargo.com/online_awb_info/index.php</t>
+  </si>
+  <si>
+    <t>https://freight.qantas.com/online-tracking.html?</t>
+  </si>
+  <si>
+    <t>http://www.qrcargo.com/trackshipment</t>
+  </si>
+  <si>
+    <t>http://www.siacargo.com/ccn/ShipmentTrack.aspx</t>
+  </si>
+  <si>
+    <t>https://www.skyteam.com/en/cargo/track-shipment/</t>
+  </si>
+  <si>
+    <t>https://www.unitedcargo.com/OurNetwork/TrackingCargo1512/Tracking.jsp</t>
+  </si>
+  <si>
+    <t>https://www.turkishcargo.com.tr/en/online-services/shipment-tracking</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -167,14 +247,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -453,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:B19"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,9 +550,11 @@
     <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="1"/>
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="159.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -476,96 +564,142 @@
       <c r="C1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1">
         <v>580</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>25</v>
       </c>
       <c r="B3" s="1">
         <v>244</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>30</v>
       </c>
       <c r="B8" s="1">
         <v>176</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>31</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>33</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -575,16 +709,22 @@
       <c r="C13" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -594,16 +734,22 @@
       <c r="C15" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>23</v>
       </c>
       <c r="B16" s="1">
         <v>157</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -613,16 +759,22 @@
       <c r="C17" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>13</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -631,16 +783,51 @@
       </c>
       <c r="C19" t="s">
         <v>28</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="A3:B15">
     <sortCondition ref="A2"/>
   </sortState>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId3" location="/tntsinglesearch"/>
+    <hyperlink ref="D5" r:id="rId4"/>
+    <hyperlink ref="D6" r:id="rId5"/>
+    <hyperlink ref="D7" r:id="rId6"/>
+    <hyperlink ref="D8" r:id="rId7"/>
+    <hyperlink ref="D9" r:id="rId8"/>
+    <hyperlink ref="D10" r:id="rId9"/>
+    <hyperlink ref="D12" r:id="rId10" location="/tntsinglesearch"/>
+    <hyperlink ref="D11" r:id="rId11"/>
+    <hyperlink ref="D13" r:id="rId12"/>
+    <hyperlink ref="D14" r:id="rId13"/>
+    <hyperlink ref="D15" r:id="rId14"/>
+    <hyperlink ref="D16" r:id="rId15"/>
+    <hyperlink ref="D17" r:id="rId16"/>
+    <hyperlink ref="D18" r:id="rId17"/>
+    <hyperlink ref="D20" r:id="rId18"/>
+    <hyperlink ref="D19" r:id="rId19"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId20"/>
   <ignoredErrors>
-    <ignoredError sqref="B20 B4 B5:B7 B9:B10 B11 B12 B13:B19" numberStoredAsText="1"/>
+    <ignoredError sqref="B4 B5:B7 B9:B10 B11 B12:B20" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Stuff for Sowrab to work on
</commit_message>
<xml_diff>
--- a/CarrierPrefixes.xlsx
+++ b/CarrierPrefixes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="82">
   <si>
     <t>Carrier</t>
   </si>
@@ -231,6 +231,45 @@
   </si>
   <si>
     <t>https://www.anacargo.jp/en/int/</t>
+  </si>
+  <si>
+    <t>Asiana</t>
+  </si>
+  <si>
+    <t>988</t>
+  </si>
+  <si>
+    <t>https://www.asianacargo.com/tracking/viewTraceAirWaybill.do?lang=en</t>
+  </si>
+  <si>
+    <t>in progress</t>
+  </si>
+  <si>
+    <t>British</t>
+  </si>
+  <si>
+    <t>125</t>
+  </si>
+  <si>
+    <t>https://www.iagcargo.com/en/home</t>
+  </si>
+  <si>
+    <t>VirginAtlantic</t>
+  </si>
+  <si>
+    <t>932</t>
+  </si>
+  <si>
+    <t>https://cargo.virgin-atlantic.com/gb/en/track/track-your-cargo.html?prefix=932&amp;number=56409673&amp;track=go</t>
+  </si>
+  <si>
+    <t>Cargolux</t>
+  </si>
+  <si>
+    <t>172</t>
+  </si>
+  <si>
+    <t>https://cvtnt.champ.aero/trackntrace</t>
   </si>
 </sst>
 </file>
@@ -563,10 +602,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -659,192 +698,248 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>69</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>42</v>
+        <v>70</v>
+      </c>
+      <c r="C7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>73</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>15</v>
+        <v>74</v>
+      </c>
+      <c r="C8" t="s">
+        <v>72</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>43</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>16</v>
+        <v>80</v>
+      </c>
+      <c r="C9" t="s">
+        <v>72</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="1">
-        <v>176</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>45</v>
+        <v>6</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
+      </c>
+      <c r="B13" s="1">
+        <v>176</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>49</v>
+        <v>17</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>50</v>
+        <v>31</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>66</v>
+        <v>32</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>67</v>
+        <v>33</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>68</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19" s="1">
-        <v>157</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>52</v>
+        <v>25</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>53</v>
+        <v>67</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>14</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" t="s">
-        <v>27</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>56</v>
+        <v>23</v>
+      </c>
+      <c r="B22" s="1">
+        <v>157</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B26" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D26" s="3" t="s">
         <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27" t="s">
+        <v>72</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -855,30 +950,34 @@
     <hyperlink ref="D2" r:id="rId1"/>
     <hyperlink ref="D3" r:id="rId2"/>
     <hyperlink ref="D4" r:id="rId3" location="/tntsinglesearch"/>
-    <hyperlink ref="D7" r:id="rId4"/>
-    <hyperlink ref="D8" r:id="rId5"/>
-    <hyperlink ref="D9" r:id="rId6"/>
-    <hyperlink ref="D10" r:id="rId7"/>
-    <hyperlink ref="D11" r:id="rId8"/>
-    <hyperlink ref="D12" r:id="rId9"/>
-    <hyperlink ref="D14" r:id="rId10" location="/tntsinglesearch"/>
-    <hyperlink ref="D13" r:id="rId11"/>
-    <hyperlink ref="D15" r:id="rId12"/>
-    <hyperlink ref="D16" r:id="rId13"/>
-    <hyperlink ref="D18" r:id="rId14"/>
-    <hyperlink ref="D19" r:id="rId15"/>
-    <hyperlink ref="D20" r:id="rId16"/>
-    <hyperlink ref="D21" r:id="rId17"/>
-    <hyperlink ref="D23" r:id="rId18"/>
-    <hyperlink ref="D22" r:id="rId19"/>
+    <hyperlink ref="D10" r:id="rId4"/>
+    <hyperlink ref="D11" r:id="rId5"/>
+    <hyperlink ref="D12" r:id="rId6"/>
+    <hyperlink ref="D13" r:id="rId7"/>
+    <hyperlink ref="D14" r:id="rId8"/>
+    <hyperlink ref="D15" r:id="rId9"/>
+    <hyperlink ref="D17" r:id="rId10" location="/tntsinglesearch"/>
+    <hyperlink ref="D16" r:id="rId11"/>
+    <hyperlink ref="D18" r:id="rId12"/>
+    <hyperlink ref="D19" r:id="rId13"/>
+    <hyperlink ref="D21" r:id="rId14"/>
+    <hyperlink ref="D22" r:id="rId15"/>
+    <hyperlink ref="D23" r:id="rId16"/>
+    <hyperlink ref="D24" r:id="rId17"/>
+    <hyperlink ref="D26" r:id="rId18"/>
+    <hyperlink ref="D25" r:id="rId19"/>
     <hyperlink ref="D5" r:id="rId20"/>
     <hyperlink ref="D6" r:id="rId21"/>
-    <hyperlink ref="D17" r:id="rId22"/>
+    <hyperlink ref="D20" r:id="rId22"/>
+    <hyperlink ref="D7" r:id="rId23"/>
+    <hyperlink ref="D8" r:id="rId24"/>
+    <hyperlink ref="D27" r:id="rId25"/>
+    <hyperlink ref="D9" r:id="rId26"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId23"/>
+  <pageSetup orientation="portrait" r:id="rId27"/>
   <ignoredErrors>
-    <ignoredError sqref="B4:B6 B7:B16 B17:B23" numberStoredAsText="1"/>
+    <ignoredError sqref="B4:B6 B7" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
removing percentage statuses for now
</commit_message>
<xml_diff>
--- a/CarrierPrefixes.xlsx
+++ b/CarrierPrefixes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="79">
   <si>
     <t>Carrier</t>
   </si>
@@ -204,15 +204,6 @@
   </si>
   <si>
     <t>https://www.aacargo.com/AACargo/tracking</t>
-  </si>
-  <si>
-    <t>about 8% can't do/cant find</t>
-  </si>
-  <si>
-    <t>about 53% done/in progress/blocked</t>
-  </si>
-  <si>
-    <t>about 39% not looked at</t>
   </si>
   <si>
     <t>https://mycargo.amerijet.com/tracking</t>
@@ -604,8 +595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -653,9 +644,6 @@
       <c r="D3" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F3" t="s">
-        <v>61</v>
-      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -667,9 +655,6 @@
       <c r="D4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F4" t="s">
-        <v>60</v>
-      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -681,61 +666,58 @@
       <c r="D5" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F5" t="s">
-        <v>62</v>
-      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" t="s">
         <v>69</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C7" t="s">
-        <v>72</v>
-      </c>
       <c r="D7" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C9" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -850,13 +832,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -930,16 +912,16 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C27" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Canada, Tampa, Swiss in progress
</commit_message>
<xml_diff>
--- a/CarrierPrefixes.xlsx
+++ b/CarrierPrefixes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="88">
   <si>
     <t>Carrier</t>
   </si>
@@ -261,6 +261,33 @@
   </si>
   <si>
     <t>https://cvtnt.champ.aero/trackntrace</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>014</t>
+  </si>
+  <si>
+    <t>https://www.aircanada.com/cargo/en/tools-forms/</t>
+  </si>
+  <si>
+    <t>Swiss</t>
+  </si>
+  <si>
+    <t>Tampa</t>
+  </si>
+  <si>
+    <t>https://www.swissworldcargo.com/track_n_trace</t>
+  </si>
+  <si>
+    <t>724</t>
+  </si>
+  <si>
+    <t>729</t>
+  </si>
+  <si>
+    <t>http://www.aviancacargo.com/index.aspx</t>
   </si>
 </sst>
 </file>
@@ -593,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B8" sqref="B8:B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,222 +723,261 @@
       <c r="B8" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C8" t="s">
-        <v>69</v>
-      </c>
       <c r="D8" s="2" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
+      </c>
+      <c r="C9" t="s">
+        <v>69</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>76</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>42</v>
+        <v>77</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>43</v>
+        <v>7</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="1">
-        <v>176</v>
+        <v>9</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>18</v>
+        <v>29</v>
+      </c>
+      <c r="B14" s="1">
+        <v>176</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>49</v>
+        <v>33</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>63</v>
+        <v>25</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>65</v>
+        <v>26</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>11</v>
+        <v>63</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>51</v>
+        <v>64</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="1">
-        <v>157</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>52</v>
+        <v>11</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>12</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>53</v>
+        <v>23</v>
+      </c>
+      <c r="B23" s="1">
+        <v>157</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C25" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>36</v>
+        <v>82</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>55</v>
+        <v>85</v>
+      </c>
+      <c r="C26" t="s">
+        <v>69</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>83</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C27" t="s">
+        <v>69</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>73</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>75</v>
       </c>
     </row>
@@ -923,34 +989,37 @@
     <hyperlink ref="D2" r:id="rId1"/>
     <hyperlink ref="D3" r:id="rId2"/>
     <hyperlink ref="D4" r:id="rId3" location="/tntsinglesearch"/>
-    <hyperlink ref="D10" r:id="rId4"/>
-    <hyperlink ref="D11" r:id="rId5"/>
-    <hyperlink ref="D12" r:id="rId6"/>
-    <hyperlink ref="D13" r:id="rId7"/>
-    <hyperlink ref="D14" r:id="rId8"/>
-    <hyperlink ref="D15" r:id="rId9"/>
-    <hyperlink ref="D17" r:id="rId10" location="/tntsinglesearch"/>
-    <hyperlink ref="D16" r:id="rId11"/>
-    <hyperlink ref="D18" r:id="rId12"/>
-    <hyperlink ref="D19" r:id="rId13"/>
-    <hyperlink ref="D21" r:id="rId14"/>
-    <hyperlink ref="D22" r:id="rId15"/>
-    <hyperlink ref="D23" r:id="rId16"/>
-    <hyperlink ref="D24" r:id="rId17"/>
-    <hyperlink ref="D26" r:id="rId18"/>
-    <hyperlink ref="D25" r:id="rId19"/>
+    <hyperlink ref="D11" r:id="rId4"/>
+    <hyperlink ref="D12" r:id="rId5"/>
+    <hyperlink ref="D13" r:id="rId6"/>
+    <hyperlink ref="D14" r:id="rId7"/>
+    <hyperlink ref="D15" r:id="rId8"/>
+    <hyperlink ref="D16" r:id="rId9"/>
+    <hyperlink ref="D18" r:id="rId10" location="/tntsinglesearch"/>
+    <hyperlink ref="D17" r:id="rId11"/>
+    <hyperlink ref="D19" r:id="rId12"/>
+    <hyperlink ref="D20" r:id="rId13"/>
+    <hyperlink ref="D22" r:id="rId14"/>
+    <hyperlink ref="D23" r:id="rId15"/>
+    <hyperlink ref="D24" r:id="rId16"/>
+    <hyperlink ref="D25" r:id="rId17"/>
+    <hyperlink ref="D29" r:id="rId18"/>
+    <hyperlink ref="D28" r:id="rId19"/>
     <hyperlink ref="D5" r:id="rId20"/>
     <hyperlink ref="D6" r:id="rId21"/>
-    <hyperlink ref="D20" r:id="rId22"/>
+    <hyperlink ref="D21" r:id="rId22"/>
     <hyperlink ref="D7" r:id="rId23"/>
     <hyperlink ref="D8" r:id="rId24"/>
-    <hyperlink ref="D27" r:id="rId25"/>
-    <hyperlink ref="D9" r:id="rId26"/>
+    <hyperlink ref="D30" r:id="rId25"/>
+    <hyperlink ref="D10" r:id="rId26"/>
+    <hyperlink ref="D9" r:id="rId27"/>
+    <hyperlink ref="D26" r:id="rId28"/>
+    <hyperlink ref="D27" r:id="rId29"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId27"/>
+  <pageSetup orientation="portrait" r:id="rId30"/>
   <ignoredErrors>
-    <ignoredError sqref="B4:B6 B7" numberStoredAsText="1"/>
+    <ignoredError sqref="B4:B6 B7 B8:B30" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Delta, ChinaCargo, ChinaSouthern, Delta in progress
</commit_message>
<xml_diff>
--- a/CarrierPrefixes.xlsx
+++ b/CarrierPrefixes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="94">
   <si>
     <t>Carrier</t>
   </si>
@@ -65,9 +65,6 @@
     <t>Singapore</t>
   </si>
   <si>
-    <t>SkyTeam</t>
-  </si>
-  <si>
     <t>Turkish</t>
   </si>
   <si>
@@ -288,6 +285,27 @@
   </si>
   <si>
     <t>http://www.aviancacargo.com/index.aspx</t>
+  </si>
+  <si>
+    <t>ChinaCargo</t>
+  </si>
+  <si>
+    <t>ChinaSouthern</t>
+  </si>
+  <si>
+    <t>784</t>
+  </si>
+  <si>
+    <t>http://tang.cs-air.com/EN/WebFace/Tang.WebFace.Cargo/AgentAwbBrower.aspx?menuID=1</t>
+  </si>
+  <si>
+    <t>Delta</t>
+  </si>
+  <si>
+    <t>006</t>
+  </si>
+  <si>
+    <t>https://www.deltacargo.com/Cargo/</t>
   </si>
 </sst>
 </file>
@@ -620,10 +638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:B30"/>
+      <selection activeCell="B15" sqref="B15:B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,10 +661,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -657,19 +675,19 @@
         <v>580</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="1">
         <v>244</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -680,76 +698,76 @@
         <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="D5" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="D6" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="D7" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="D8" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="C9" t="s">
-        <v>69</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="D10" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -760,7 +778,7 @@
         <v>7</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -768,217 +786,245 @@
         <v>8</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>87</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>44</v>
+        <v>20</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="1">
-        <v>176</v>
+        <v>88</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C14" t="s">
+        <v>68</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>45</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>18</v>
+        <v>92</v>
+      </c>
+      <c r="C15" t="s">
+        <v>68</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>46</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
+      </c>
+      <c r="B17" s="1">
+        <v>176</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>49</v>
+        <v>16</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>50</v>
+        <v>30</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>63</v>
+        <v>31</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="1">
-        <v>157</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>52</v>
+        <v>24</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>12</v>
+        <v>62</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>53</v>
+        <v>63</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>82</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C26" t="s">
-        <v>69</v>
+        <v>22</v>
+      </c>
+      <c r="B26" s="1">
+        <v>157</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>84</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>83</v>
+        <v>12</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C27" t="s">
-        <v>69</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>87</v>
+        <v>19</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>14</v>
+        <v>81</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>22</v>
+        <v>84</v>
       </c>
       <c r="C28" t="s">
-        <v>27</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>56</v>
+        <v>68</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>36</v>
+        <v>82</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>55</v>
+        <v>85</v>
+      </c>
+      <c r="C29" t="s">
+        <v>68</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>72</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="D32" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -991,35 +1037,37 @@
     <hyperlink ref="D4" r:id="rId3" location="/tntsinglesearch"/>
     <hyperlink ref="D11" r:id="rId4"/>
     <hyperlink ref="D12" r:id="rId5"/>
-    <hyperlink ref="D13" r:id="rId6"/>
-    <hyperlink ref="D14" r:id="rId7"/>
-    <hyperlink ref="D15" r:id="rId8"/>
-    <hyperlink ref="D16" r:id="rId9"/>
-    <hyperlink ref="D18" r:id="rId10" location="/tntsinglesearch"/>
-    <hyperlink ref="D17" r:id="rId11"/>
-    <hyperlink ref="D19" r:id="rId12"/>
-    <hyperlink ref="D20" r:id="rId13"/>
-    <hyperlink ref="D22" r:id="rId14"/>
-    <hyperlink ref="D23" r:id="rId15"/>
-    <hyperlink ref="D24" r:id="rId16"/>
-    <hyperlink ref="D25" r:id="rId17"/>
-    <hyperlink ref="D29" r:id="rId18"/>
-    <hyperlink ref="D28" r:id="rId19"/>
+    <hyperlink ref="D16" r:id="rId6"/>
+    <hyperlink ref="D17" r:id="rId7"/>
+    <hyperlink ref="D18" r:id="rId8"/>
+    <hyperlink ref="D19" r:id="rId9"/>
+    <hyperlink ref="D21" r:id="rId10" location="/tntsinglesearch"/>
+    <hyperlink ref="D20" r:id="rId11"/>
+    <hyperlink ref="D22" r:id="rId12"/>
+    <hyperlink ref="D23" r:id="rId13"/>
+    <hyperlink ref="D25" r:id="rId14"/>
+    <hyperlink ref="D26" r:id="rId15"/>
+    <hyperlink ref="D27" r:id="rId16"/>
+    <hyperlink ref="D13" r:id="rId17"/>
+    <hyperlink ref="D31" r:id="rId18"/>
+    <hyperlink ref="D30" r:id="rId19"/>
     <hyperlink ref="D5" r:id="rId20"/>
     <hyperlink ref="D6" r:id="rId21"/>
-    <hyperlink ref="D21" r:id="rId22"/>
+    <hyperlink ref="D24" r:id="rId22"/>
     <hyperlink ref="D7" r:id="rId23"/>
     <hyperlink ref="D8" r:id="rId24"/>
-    <hyperlink ref="D30" r:id="rId25"/>
+    <hyperlink ref="D32" r:id="rId25"/>
     <hyperlink ref="D10" r:id="rId26"/>
     <hyperlink ref="D9" r:id="rId27"/>
-    <hyperlink ref="D26" r:id="rId28"/>
-    <hyperlink ref="D27" r:id="rId29"/>
+    <hyperlink ref="D28" r:id="rId28"/>
+    <hyperlink ref="D29" r:id="rId29"/>
+    <hyperlink ref="D14" r:id="rId30"/>
+    <hyperlink ref="D15" r:id="rId31"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId30"/>
+  <pageSetup orientation="portrait" r:id="rId32"/>
   <ignoredErrors>
-    <ignoredError sqref="B4:B6 B7 B8:B30" numberStoredAsText="1"/>
+    <ignoredError sqref="B4:B6 B7 B8:B12 B13:B14 B15:B32" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Scandinavian in progress + mappings
</commit_message>
<xml_diff>
--- a/CarrierPrefixes.xlsx
+++ b/CarrierPrefixes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="96">
   <si>
     <t>Carrier</t>
   </si>
@@ -306,6 +306,12 @@
   </si>
   <si>
     <t>https://www.deltacargo.com/Cargo/</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Mapping Done?</t>
   </si>
 </sst>
 </file>
@@ -641,7 +647,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:B32"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -650,6 +656,7 @@
     <col min="2" max="2" width="9.140625" style="1"/>
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="159.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -666,6 +673,9 @@
       <c r="D1" t="s">
         <v>37</v>
       </c>
+      <c r="E1" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -677,6 +687,9 @@
       <c r="D2" s="2" t="s">
         <v>38</v>
       </c>
+      <c r="E2" t="s">
+        <v>94</v>
+      </c>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -689,6 +702,9 @@
       <c r="D3" s="3" t="s">
         <v>40</v>
       </c>
+      <c r="E3" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -700,6 +716,9 @@
       <c r="D4" s="2" t="s">
         <v>39</v>
       </c>
+      <c r="E4" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -780,6 +799,9 @@
       <c r="D11" s="3" t="s">
         <v>41</v>
       </c>
+      <c r="E11" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -791,6 +813,9 @@
       <c r="D12" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="E12" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -842,7 +867,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -852,8 +877,11 @@
       <c r="D17" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -863,8 +891,11 @@
       <c r="D18" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -874,8 +905,11 @@
       <c r="D19" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -886,7 +920,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -896,8 +930,11 @@
       <c r="D21" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -908,7 +945,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -919,7 +956,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>62</v>
       </c>
@@ -930,7 +967,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>11</v>
       </c>
@@ -941,7 +978,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -952,7 +989,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -963,7 +1000,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>81</v>
       </c>
@@ -977,7 +1014,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>82</v>
       </c>
@@ -991,7 +1028,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>13</v>
       </c>
@@ -1004,8 +1041,11 @@
       <c r="D30" s="3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -1016,7 +1056,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>72</v>
       </c>

</xml_diff>

<commit_message>
small fix to cargo handlers
</commit_message>
<xml_diff>
--- a/CarrierPrefixes.xlsx
+++ b/CarrierPrefixes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="99">
   <si>
     <t>Carrier</t>
   </si>
@@ -50,9 +50,6 @@
     <t>160</t>
   </si>
   <si>
-    <t>China</t>
-  </si>
-  <si>
     <t>DHL</t>
   </si>
   <si>
@@ -312,6 +309,18 @@
   </si>
   <si>
     <t>Mapping Done?</t>
+  </si>
+  <si>
+    <t>ChinaAirlines</t>
+  </si>
+  <si>
+    <t>AirChina</t>
+  </si>
+  <si>
+    <t>999</t>
+  </si>
+  <si>
+    <t>http://www.airchinacargo.com/en/index.php?section=0-0149-0154</t>
   </si>
 </sst>
 </file>
@@ -644,10 +653,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -668,13 +677,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -685,429 +694,435 @@
         <v>580</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="1">
-        <v>244</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E3" t="s">
-        <v>94</v>
+        <v>96</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="1">
+        <v>244</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>39</v>
       </c>
       <c r="E4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>57</v>
+        <v>5</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>58</v>
+        <v>38</v>
+      </c>
+      <c r="E5" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
+      </c>
+      <c r="C10" t="s">
+        <v>67</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>74</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E11" t="s">
-        <v>94</v>
+        <v>75</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>42</v>
+        <v>7</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="E12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>53</v>
+        <v>13</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C14" t="s">
-        <v>68</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>90</v>
+        <v>19</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>90</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>15</v>
+        <v>91</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>43</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="1">
-        <v>176</v>
+        <v>8</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E17" t="s">
-        <v>94</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
+      </c>
+      <c r="B18" s="1">
+        <v>176</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
+      </c>
+      <c r="E20" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E21" t="s">
-        <v>94</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>48</v>
+        <v>31</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>62</v>
+        <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>64</v>
+        <v>24</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>11</v>
+        <v>61</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>50</v>
+        <v>62</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>22</v>
-      </c>
-      <c r="B26" s="1">
-        <v>157</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>51</v>
+        <v>10</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>12</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>52</v>
+        <v>21</v>
+      </c>
+      <c r="B27" s="1">
+        <v>157</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>81</v>
+        <v>11</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C28" t="s">
-        <v>68</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>83</v>
+        <v>18</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>80</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C29" t="s">
-        <v>68</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>13</v>
+        <v>81</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>21</v>
+        <v>84</v>
       </c>
       <c r="C30" t="s">
-        <v>26</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E30" t="s">
-        <v>94</v>
+        <v>67</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>36</v>
+        <v>20</v>
+      </c>
+      <c r="C31" t="s">
+        <v>25</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>54</v>
       </c>
+      <c r="E31" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>71</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="D33" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>74</v>
-      </c>
     </row>
   </sheetData>
-  <sortState ref="A3:B15">
+  <sortState ref="A4:B16">
     <sortCondition ref="A2"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="D4" r:id="rId3" location="/tntsinglesearch"/>
-    <hyperlink ref="D11" r:id="rId4"/>
-    <hyperlink ref="D12" r:id="rId5"/>
-    <hyperlink ref="D16" r:id="rId6"/>
-    <hyperlink ref="D17" r:id="rId7"/>
-    <hyperlink ref="D18" r:id="rId8"/>
-    <hyperlink ref="D19" r:id="rId9"/>
-    <hyperlink ref="D21" r:id="rId10" location="/tntsinglesearch"/>
-    <hyperlink ref="D20" r:id="rId11"/>
-    <hyperlink ref="D22" r:id="rId12"/>
-    <hyperlink ref="D23" r:id="rId13"/>
-    <hyperlink ref="D25" r:id="rId14"/>
-    <hyperlink ref="D26" r:id="rId15"/>
-    <hyperlink ref="D27" r:id="rId16"/>
-    <hyperlink ref="D13" r:id="rId17"/>
-    <hyperlink ref="D31" r:id="rId18"/>
-    <hyperlink ref="D30" r:id="rId19"/>
-    <hyperlink ref="D5" r:id="rId20"/>
-    <hyperlink ref="D6" r:id="rId21"/>
-    <hyperlink ref="D24" r:id="rId22"/>
-    <hyperlink ref="D7" r:id="rId23"/>
-    <hyperlink ref="D8" r:id="rId24"/>
-    <hyperlink ref="D32" r:id="rId25"/>
-    <hyperlink ref="D10" r:id="rId26"/>
-    <hyperlink ref="D9" r:id="rId27"/>
-    <hyperlink ref="D28" r:id="rId28"/>
-    <hyperlink ref="D29" r:id="rId29"/>
-    <hyperlink ref="D14" r:id="rId30"/>
-    <hyperlink ref="D15" r:id="rId31"/>
+    <hyperlink ref="D4" r:id="rId2"/>
+    <hyperlink ref="D5" r:id="rId3" location="/tntsinglesearch"/>
+    <hyperlink ref="D12" r:id="rId4"/>
+    <hyperlink ref="D13" r:id="rId5"/>
+    <hyperlink ref="D17" r:id="rId6"/>
+    <hyperlink ref="D18" r:id="rId7"/>
+    <hyperlink ref="D19" r:id="rId8"/>
+    <hyperlink ref="D20" r:id="rId9"/>
+    <hyperlink ref="D22" r:id="rId10" location="/tntsinglesearch"/>
+    <hyperlink ref="D21" r:id="rId11"/>
+    <hyperlink ref="D23" r:id="rId12"/>
+    <hyperlink ref="D24" r:id="rId13"/>
+    <hyperlink ref="D26" r:id="rId14"/>
+    <hyperlink ref="D27" r:id="rId15"/>
+    <hyperlink ref="D28" r:id="rId16"/>
+    <hyperlink ref="D14" r:id="rId17"/>
+    <hyperlink ref="D32" r:id="rId18"/>
+    <hyperlink ref="D31" r:id="rId19"/>
+    <hyperlink ref="D6" r:id="rId20"/>
+    <hyperlink ref="D7" r:id="rId21"/>
+    <hyperlink ref="D25" r:id="rId22"/>
+    <hyperlink ref="D8" r:id="rId23"/>
+    <hyperlink ref="D9" r:id="rId24"/>
+    <hyperlink ref="D33" r:id="rId25"/>
+    <hyperlink ref="D11" r:id="rId26"/>
+    <hyperlink ref="D10" r:id="rId27"/>
+    <hyperlink ref="D29" r:id="rId28"/>
+    <hyperlink ref="D30" r:id="rId29"/>
+    <hyperlink ref="D15" r:id="rId30"/>
+    <hyperlink ref="D16" r:id="rId31"/>
+    <hyperlink ref="D3" r:id="rId32"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId32"/>
-  <ignoredErrors>
-    <ignoredError sqref="B4:B6 B7 B8:B12 B13:B14 B15:B32" numberStoredAsText="1"/>
-  </ignoredErrors>
+  <pageSetup orientation="portrait" r:id="rId33"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added RPA part and updated handlers for all terminals
</commit_message>
<xml_diff>
--- a/CarrierPrefixes.xlsx
+++ b/CarrierPrefixes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pvanausdeln\Dropbox (Blume Global)\Documents\UiPath\AirCarrierRPA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Blume-proj\AirCarrierRPA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="102">
   <si>
     <t>Carrier</t>
   </si>
@@ -227,9 +227,6 @@
     <t>https://www.asianacargo.com/tracking/viewTraceAirWaybill.do?lang=en</t>
   </si>
   <si>
-    <t>in progress</t>
-  </si>
-  <si>
     <t>British</t>
   </si>
   <si>
@@ -321,6 +318,18 @@
   </si>
   <si>
     <t>http://www.airchinacargo.com/en/index.php?section=0-0149-0154</t>
+  </si>
+  <si>
+    <t>Scandavian</t>
+  </si>
+  <si>
+    <t>117</t>
+  </si>
+  <si>
+    <t>https://www.sascargo.com/en/Booking/Track-Shipment.aspx</t>
+  </si>
+  <si>
+    <t>In Progress</t>
   </si>
 </sst>
 </file>
@@ -653,10 +662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,7 +692,7 @@
         <v>36</v>
       </c>
       <c r="E1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -697,22 +706,22 @@
         <v>37</v>
       </c>
       <c r="E2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="C3" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -726,7 +735,7 @@
         <v>39</v>
       </c>
       <c r="E4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -740,7 +749,7 @@
         <v>38</v>
       </c>
       <c r="E5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -778,38 +787,35 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="D9" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="D10" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="C10" t="s">
-        <v>67</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="D11" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -823,12 +829,12 @@
         <v>40</v>
       </c>
       <c r="E12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>13</v>
@@ -837,12 +843,12 @@
         <v>41</v>
       </c>
       <c r="E13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>19</v>
@@ -853,27 +859,24 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="D15" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="C15" t="s">
-        <v>67</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="D16" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -898,7 +901,7 @@
         <v>43</v>
       </c>
       <c r="E18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -912,7 +915,7 @@
         <v>44</v>
       </c>
       <c r="E19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -926,7 +929,7 @@
         <v>45</v>
       </c>
       <c r="E20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -951,7 +954,7 @@
         <v>38</v>
       </c>
       <c r="E22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1022,27 +1025,24 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="C30" t="s">
-        <v>67</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1059,7 +1059,7 @@
         <v>54</v>
       </c>
       <c r="E31" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1075,13 +1075,27 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>70</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="D33" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>73</v>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>98</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C34" t="s">
+        <v>101</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1121,8 +1135,9 @@
     <hyperlink ref="D15" r:id="rId30"/>
     <hyperlink ref="D16" r:id="rId31"/>
     <hyperlink ref="D3" r:id="rId32"/>
+    <hyperlink ref="D34" r:id="rId33"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId33"/>
+  <pageSetup orientation="portrait" r:id="rId34"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updates to statuses and prefixes
</commit_message>
<xml_diff>
--- a/CarrierPrefixes.xlsx
+++ b/CarrierPrefixes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Blume-proj\AirCarrierRPA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pvanausdeln\Dropbox (Blume Global)\Documents\UiPath\AirCarrierRPA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="132">
   <si>
     <t>Carrier</t>
   </si>
@@ -92,21 +92,12 @@
     <t>Qatar</t>
   </si>
   <si>
-    <t>Air Tahiti</t>
-  </si>
-  <si>
     <t>MalaysiaCargo</t>
   </si>
   <si>
     <t>232</t>
   </si>
   <si>
-    <t>Blocked</t>
-  </si>
-  <si>
-    <t>RPA Status</t>
-  </si>
-  <si>
     <t>EmiratesSky</t>
   </si>
   <si>
@@ -302,12 +293,6 @@
     <t>https://www.deltacargo.com/Cargo/</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>Mapping Done?</t>
-  </si>
-  <si>
     <t>ChinaAirlines</t>
   </si>
   <si>
@@ -329,14 +314,119 @@
     <t>https://www.sascargo.com/en/Booking/Track-Shipment.aspx</t>
   </si>
   <si>
-    <t>In Progress</t>
+    <t>AirTahiti</t>
+  </si>
+  <si>
+    <t>AerLingus</t>
+  </si>
+  <si>
+    <t>053</t>
+  </si>
+  <si>
+    <t>AirIndia</t>
+  </si>
+  <si>
+    <t>http://www.airindia.in/cargo-tracking.htm</t>
+  </si>
+  <si>
+    <t>098</t>
+  </si>
+  <si>
+    <t>Etihad</t>
+  </si>
+  <si>
+    <t>ChinaEastern</t>
+  </si>
+  <si>
+    <t>781</t>
+  </si>
+  <si>
+    <t>607</t>
+  </si>
+  <si>
+    <t>https://www.etihadcargo.com/en-ae/track-and-trace.html</t>
+  </si>
+  <si>
+    <t>cannot find the site</t>
+  </si>
+  <si>
+    <t>Fedex</t>
+  </si>
+  <si>
+    <t>https://www.fedex.com/en-ca/home.html</t>
+  </si>
+  <si>
+    <t>023</t>
+  </si>
+  <si>
+    <t>Hainan</t>
+  </si>
+  <si>
+    <t>Iberian</t>
+  </si>
+  <si>
+    <t>LOT Polish</t>
+  </si>
+  <si>
+    <t>Norwegian</t>
+  </si>
+  <si>
+    <t>Phillipines</t>
+  </si>
+  <si>
+    <t>SkyLease</t>
+  </si>
+  <si>
+    <t>576</t>
+  </si>
+  <si>
+    <t>http://www.skyleasecargo.com/</t>
+  </si>
+  <si>
+    <t>Solar</t>
+  </si>
+  <si>
+    <t>880</t>
+  </si>
+  <si>
+    <t>http://www.hnacargo.com/Portal2/AwbSearch.aspx</t>
+  </si>
+  <si>
+    <t>075</t>
+  </si>
+  <si>
+    <t>080</t>
+  </si>
+  <si>
+    <t>http://cargoserv.champ.aero/tracking.asp?Carrier=LO&amp;Pfx=080</t>
+  </si>
+  <si>
+    <t>079</t>
+  </si>
+  <si>
+    <t>http://cargoserv.champ.aero/tracking.asp?Carrier=PR&amp;Pfx=079</t>
+  </si>
+  <si>
+    <t>https://www.norwegiancargo.com/</t>
+  </si>
+  <si>
+    <t>http://sc.cargolink.aero/Cargolinktracking/</t>
+  </si>
+  <si>
+    <t>644</t>
+  </si>
+  <si>
+    <t>328</t>
+  </si>
+  <si>
+    <t>not OL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -352,13 +442,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -370,20 +472,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -662,20 +771,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="159.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="138.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" customWidth="1"/>
+    <col min="6" max="6" width="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -686,55 +795,40 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1">
-        <v>580</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" t="s">
-        <v>92</v>
+        <v>97</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>97</v>
+        <v>3</v>
+      </c>
+      <c r="B3" s="1">
+        <v>580</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="1">
-        <v>244</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>92</v>
       </c>
     </row>
@@ -745,399 +839,524 @@
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" t="s">
-        <v>92</v>
+      <c r="C5" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>99</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>57</v>
+        <v>101</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>59</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>58</v>
+      <c r="A7" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" s="5">
+        <v>244</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>66</v>
+        <v>53</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>69</v>
+        <v>57</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>78</v>
+        <v>62</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B12" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="C12" s="4" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" t="s">
-        <v>92</v>
+      <c r="D12" s="4" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" t="s">
-        <v>92</v>
+        <v>71</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>85</v>
+        <v>6</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>52</v>
+        <v>7</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>88</v>
+        <v>13</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>103</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>83</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>86</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B20" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="C20" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="1">
+        <v>176</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>102</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>108</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>111</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>112</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="1">
-        <v>176</v>
-      </c>
-      <c r="D18" s="2" t="s">
+      <c r="B28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>113</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E18" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E19" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>2</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" s="2" t="s">
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>22</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E20" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D21" s="2" t="s">
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>58</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>114</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>115</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>10</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22" s="1" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>21</v>
+      </c>
+      <c r="B37" s="1">
+        <v>157</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>93</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>11</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>116</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>119</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>76</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>77</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E22" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="B45" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>61</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>10</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>21</v>
-      </c>
-      <c r="B27" s="1">
-        <v>157</v>
-      </c>
-      <c r="D27" s="2" t="s">
+      <c r="C45" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>11</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>79</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>80</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>12</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C31" t="s">
-        <v>25</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E31" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>34</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>70</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>98</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C34" t="s">
-        <v>101</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>100</v>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>67</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A4:B16">
+  <sortState ref="A3:E35">
     <sortCondition ref="A2"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D4" r:id="rId2"/>
-    <hyperlink ref="D5" r:id="rId3" location="/tntsinglesearch"/>
-    <hyperlink ref="D12" r:id="rId4"/>
-    <hyperlink ref="D13" r:id="rId5"/>
-    <hyperlink ref="D17" r:id="rId6"/>
-    <hyperlink ref="D18" r:id="rId7"/>
-    <hyperlink ref="D19" r:id="rId8"/>
-    <hyperlink ref="D20" r:id="rId9"/>
-    <hyperlink ref="D22" r:id="rId10" location="/tntsinglesearch"/>
-    <hyperlink ref="D21" r:id="rId11"/>
-    <hyperlink ref="D23" r:id="rId12"/>
-    <hyperlink ref="D24" r:id="rId13"/>
-    <hyperlink ref="D26" r:id="rId14"/>
-    <hyperlink ref="D27" r:id="rId15"/>
-    <hyperlink ref="D28" r:id="rId16"/>
-    <hyperlink ref="D14" r:id="rId17"/>
-    <hyperlink ref="D32" r:id="rId18"/>
-    <hyperlink ref="D31" r:id="rId19"/>
-    <hyperlink ref="D6" r:id="rId20"/>
-    <hyperlink ref="D7" r:id="rId21"/>
-    <hyperlink ref="D25" r:id="rId22"/>
-    <hyperlink ref="D8" r:id="rId23"/>
-    <hyperlink ref="D9" r:id="rId24"/>
-    <hyperlink ref="D33" r:id="rId25"/>
-    <hyperlink ref="D11" r:id="rId26"/>
-    <hyperlink ref="D10" r:id="rId27"/>
-    <hyperlink ref="D29" r:id="rId28"/>
-    <hyperlink ref="D30" r:id="rId29"/>
-    <hyperlink ref="D15" r:id="rId30"/>
-    <hyperlink ref="D16" r:id="rId31"/>
-    <hyperlink ref="D3" r:id="rId32"/>
-    <hyperlink ref="D34" r:id="rId33"/>
+    <hyperlink ref="C3" r:id="rId1"/>
+    <hyperlink ref="C7" r:id="rId2"/>
+    <hyperlink ref="C5" r:id="rId3" location="/tntsinglesearch"/>
+    <hyperlink ref="C14" r:id="rId4"/>
+    <hyperlink ref="C15" r:id="rId5"/>
+    <hyperlink ref="C20" r:id="rId6"/>
+    <hyperlink ref="C21" r:id="rId7"/>
+    <hyperlink ref="C23" r:id="rId8"/>
+    <hyperlink ref="C27" r:id="rId9"/>
+    <hyperlink ref="C28" r:id="rId10" location="/tntsinglesearch"/>
+    <hyperlink ref="C31" r:id="rId11"/>
+    <hyperlink ref="C29" r:id="rId12"/>
+    <hyperlink ref="C32" r:id="rId13"/>
+    <hyperlink ref="C36" r:id="rId14"/>
+    <hyperlink ref="C37" r:id="rId15"/>
+    <hyperlink ref="C39" r:id="rId16"/>
+    <hyperlink ref="C16" r:id="rId17"/>
+    <hyperlink ref="C45" r:id="rId18"/>
+    <hyperlink ref="C44" r:id="rId19"/>
+    <hyperlink ref="C8" r:id="rId20"/>
+    <hyperlink ref="C9" r:id="rId21"/>
+    <hyperlink ref="C33" r:id="rId22"/>
+    <hyperlink ref="C10" r:id="rId23"/>
+    <hyperlink ref="C11" r:id="rId24"/>
+    <hyperlink ref="C46" r:id="rId25"/>
+    <hyperlink ref="C13" r:id="rId26"/>
+    <hyperlink ref="C12" r:id="rId27"/>
+    <hyperlink ref="C42" r:id="rId28"/>
+    <hyperlink ref="C43" r:id="rId29"/>
+    <hyperlink ref="C18" r:id="rId30"/>
+    <hyperlink ref="C19" r:id="rId31"/>
+    <hyperlink ref="C4" r:id="rId32"/>
+    <hyperlink ref="C38" r:id="rId33"/>
+    <hyperlink ref="C2" r:id="rId34"/>
+    <hyperlink ref="C6" r:id="rId35"/>
+    <hyperlink ref="C22" r:id="rId36"/>
+    <hyperlink ref="C24" r:id="rId37"/>
+    <hyperlink ref="C40" r:id="rId38"/>
+    <hyperlink ref="C25" r:id="rId39"/>
+    <hyperlink ref="C26" r:id="rId40"/>
+    <hyperlink ref="C30" r:id="rId41"/>
+    <hyperlink ref="C35" r:id="rId42"/>
+    <hyperlink ref="C34" r:id="rId43"/>
+    <hyperlink ref="C41" r:id="rId44"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId34"/>
+  <pageSetup orientation="portrait" r:id="rId45"/>
+  <ignoredErrors>
+    <ignoredError sqref="B2:B33 B35:B46" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
prefix and mapping updates
</commit_message>
<xml_diff>
--- a/CarrierPrefixes.xlsx
+++ b/CarrierPrefixes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="135">
   <si>
     <t>Carrier</t>
   </si>
@@ -245,9 +245,6 @@
     <t>https://cvtnt.champ.aero/trackntrace</t>
   </si>
   <si>
-    <t>Canada</t>
-  </si>
-  <si>
     <t>014</t>
   </si>
   <si>
@@ -420,6 +417,18 @@
   </si>
   <si>
     <t>not OL</t>
+  </si>
+  <si>
+    <t>AirCanada</t>
+  </si>
+  <si>
+    <t>ANANippon</t>
+  </si>
+  <si>
+    <t>933</t>
+  </si>
+  <si>
+    <t>https://www.nca.aero/icargoportal/portal/trackshipments?</t>
   </si>
 </sst>
 </file>
@@ -771,10 +780,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="B2" sqref="B2:B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -800,10 +809,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>66</v>
@@ -823,540 +832,555 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>90</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>91</v>
+        <v>131</v>
+      </c>
+      <c r="B4" t="s">
+        <v>73</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>89</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>5</v>
+        <v>90</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>35</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B7" s="5">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" s="5">
         <v>244</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C8" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>52</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>54</v>
+      <c r="D8" s="4" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>64</v>
+        <v>132</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>131</v>
+      <c r="A12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>70</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>37</v>
+        <v>71</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>89</v>
+        <v>6</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>38</v>
+        <v>7</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>49</v>
+        <v>13</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C17" t="s">
-        <v>107</v>
+        <v>19</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>83</v>
+        <v>102</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>85</v>
+        <v>103</v>
+      </c>
+      <c r="C18" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>82</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>85</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C20" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B21" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C21" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" s="1">
-        <v>176</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>40</v>
+      <c r="D21" s="4" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>102</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>105</v>
+        <v>24</v>
+      </c>
+      <c r="B22" s="1">
+        <v>176</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>106</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>101</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B24" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C24" s="4" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>108</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>109</v>
+      <c r="D24" s="4" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>66</v>
+        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>2</v>
+        <v>111</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>15</v>
+        <v>121</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>44</v>
+        <v>28</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>113</v>
+        <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>124</v>
+        <v>30</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>25</v>
+        <v>112</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>26</v>
+        <v>122</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>43</v>
+        <v>123</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B33" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C33" s="6" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="D33" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>58</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>114</v>
-      </c>
       <c r="B34" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>114</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>10</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B37" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C37" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>21</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B38" s="1">
         <v>157</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C38" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>92</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="C39" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C38" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>11</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B40" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C40" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>115</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="C41" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="C40" s="2" t="s">
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>119</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C41" s="2" t="s">
+      <c r="B42" s="1" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="C42" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>75</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>76</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B44" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C42" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>77</v>
-      </c>
-      <c r="B43" s="1" t="s">
+      <c r="C44" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C43" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>12</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C45" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>31</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B46" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C46" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>67</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B47" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C47" s="2" t="s">
         <v>69</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A3:E35">
+  <sortState ref="A2:D46">
     <sortCondition ref="A2"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1"/>
-    <hyperlink ref="C7" r:id="rId2"/>
-    <hyperlink ref="C5" r:id="rId3" location="/tntsinglesearch"/>
-    <hyperlink ref="C14" r:id="rId4"/>
-    <hyperlink ref="C15" r:id="rId5"/>
-    <hyperlink ref="C20" r:id="rId6"/>
-    <hyperlink ref="C21" r:id="rId7"/>
-    <hyperlink ref="C23" r:id="rId8"/>
-    <hyperlink ref="C27" r:id="rId9"/>
-    <hyperlink ref="C28" r:id="rId10" location="/tntsinglesearch"/>
-    <hyperlink ref="C31" r:id="rId11"/>
-    <hyperlink ref="C29" r:id="rId12"/>
-    <hyperlink ref="C32" r:id="rId13"/>
-    <hyperlink ref="C36" r:id="rId14"/>
-    <hyperlink ref="C37" r:id="rId15"/>
-    <hyperlink ref="C39" r:id="rId16"/>
-    <hyperlink ref="C16" r:id="rId17"/>
-    <hyperlink ref="C45" r:id="rId18"/>
-    <hyperlink ref="C44" r:id="rId19"/>
-    <hyperlink ref="C8" r:id="rId20"/>
-    <hyperlink ref="C9" r:id="rId21"/>
-    <hyperlink ref="C33" r:id="rId22"/>
-    <hyperlink ref="C10" r:id="rId23"/>
-    <hyperlink ref="C11" r:id="rId24"/>
-    <hyperlink ref="C46" r:id="rId25"/>
-    <hyperlink ref="C13" r:id="rId26"/>
-    <hyperlink ref="C12" r:id="rId27"/>
-    <hyperlink ref="C42" r:id="rId28"/>
-    <hyperlink ref="C43" r:id="rId29"/>
-    <hyperlink ref="C18" r:id="rId30"/>
-    <hyperlink ref="C19" r:id="rId31"/>
-    <hyperlink ref="C4" r:id="rId32"/>
-    <hyperlink ref="C38" r:id="rId33"/>
+    <hyperlink ref="C8" r:id="rId2"/>
+    <hyperlink ref="C6" r:id="rId3" location="/tntsinglesearch"/>
+    <hyperlink ref="C15" r:id="rId4"/>
+    <hyperlink ref="C16" r:id="rId5"/>
+    <hyperlink ref="C21" r:id="rId6"/>
+    <hyperlink ref="C22" r:id="rId7"/>
+    <hyperlink ref="C24" r:id="rId8"/>
+    <hyperlink ref="C28" r:id="rId9"/>
+    <hyperlink ref="C29" r:id="rId10" location="/tntsinglesearch"/>
+    <hyperlink ref="C32" r:id="rId11"/>
+    <hyperlink ref="C30" r:id="rId12"/>
+    <hyperlink ref="C33" r:id="rId13"/>
+    <hyperlink ref="C37" r:id="rId14"/>
+    <hyperlink ref="C38" r:id="rId15"/>
+    <hyperlink ref="C40" r:id="rId16"/>
+    <hyperlink ref="C17" r:id="rId17"/>
+    <hyperlink ref="C46" r:id="rId18"/>
+    <hyperlink ref="C45" r:id="rId19"/>
+    <hyperlink ref="C9" r:id="rId20"/>
+    <hyperlink ref="C10" r:id="rId21"/>
+    <hyperlink ref="C11" r:id="rId22"/>
+    <hyperlink ref="C12" r:id="rId23"/>
+    <hyperlink ref="C13" r:id="rId24"/>
+    <hyperlink ref="C47" r:id="rId25"/>
+    <hyperlink ref="C14" r:id="rId26"/>
+    <hyperlink ref="C4" r:id="rId27"/>
+    <hyperlink ref="C43" r:id="rId28"/>
+    <hyperlink ref="C44" r:id="rId29"/>
+    <hyperlink ref="C19" r:id="rId30"/>
+    <hyperlink ref="C20" r:id="rId31"/>
+    <hyperlink ref="C5" r:id="rId32"/>
+    <hyperlink ref="C39" r:id="rId33"/>
     <hyperlink ref="C2" r:id="rId34"/>
-    <hyperlink ref="C6" r:id="rId35"/>
-    <hyperlink ref="C22" r:id="rId36"/>
-    <hyperlink ref="C24" r:id="rId37"/>
-    <hyperlink ref="C40" r:id="rId38"/>
-    <hyperlink ref="C25" r:id="rId39"/>
-    <hyperlink ref="C26" r:id="rId40"/>
-    <hyperlink ref="C30" r:id="rId41"/>
-    <hyperlink ref="C35" r:id="rId42"/>
-    <hyperlink ref="C34" r:id="rId43"/>
-    <hyperlink ref="C41" r:id="rId44"/>
+    <hyperlink ref="C7" r:id="rId35"/>
+    <hyperlink ref="C23" r:id="rId36"/>
+    <hyperlink ref="C25" r:id="rId37"/>
+    <hyperlink ref="C41" r:id="rId38"/>
+    <hyperlink ref="C26" r:id="rId39"/>
+    <hyperlink ref="C27" r:id="rId40"/>
+    <hyperlink ref="C31" r:id="rId41"/>
+    <hyperlink ref="C36" r:id="rId42"/>
+    <hyperlink ref="C35" r:id="rId43"/>
+    <hyperlink ref="C42" r:id="rId44"/>
+    <hyperlink ref="C34" r:id="rId45"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId45"/>
+  <pageSetup orientation="portrait" r:id="rId46"/>
   <ignoredErrors>
-    <ignoredError sqref="B2:B33 B35:B46" numberStoredAsText="1"/>
+    <ignoredError sqref="B2:B47" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>